<commit_message>
Added Model Fitting Notebook
This notebook contains BUZEN's algorithm runs for each scenario, configuration and clients configuration
</commit_message>
<xml_diff>
--- a/excel/BuzenConvolutionAlgorithm.xlsx
+++ b/excel/BuzenConvolutionAlgorithm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pecsn_project\pecsn_project\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA949DCC-E29A-415F-9E7B-35244E215D72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6120BA3D-DF45-4899-BD1F-793BB94E59A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,12 +474,13 @@
   <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -619,31 +620,31 @@
         <v>1</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" ref="K5:K36" si="1">N5*$I5/$I$55</f>
-        <v>1.6355545122680336E-28</v>
+        <f>N5*$I5/$I$54</f>
+        <v>5.5062233882749881E-28</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" ref="L5:L36" si="2">O5*$I5/$I$55</f>
-        <v>1.378357956173948E-2</v>
+        <f t="shared" ref="L5:M20" si="1">O5*$I5/$I$54</f>
+        <v>1.4061669324827207E-2</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" ref="M5:M36" si="3">P5*$I5/$I$55</f>
-        <v>1.378357956173948E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4061669324827207E-2</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" ref="N5:N36" si="4">POWER(G$2,$Q5)</f>
+        <f>POWER(G$2,$Q5)</f>
         <v>1</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" ref="O5:O36" si="5">POWER(H$2,$Q5)</f>
-        <v>8.427465705576334E+25</v>
+        <f>POWER(H$2,$Q5)</f>
+        <v>2.5537774865382829E+25</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" ref="P5:P36" si="6">POWER(I$2,$Q5)</f>
-        <v>8.427465705576334E+25</v>
+        <f>POWER(I$2,$Q5)</f>
+        <v>2.5537774865382829E+25</v>
       </c>
       <c r="Q5" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
@@ -654,19 +655,19 @@
         <v>16</v>
       </c>
       <c r="B6" s="1">
-        <f>G2*$I$54/$I$55</f>
-        <v>0.29703744235128587</v>
+        <f>G2*$I$53/$I$54</f>
+        <v>0.29691653375863908</v>
       </c>
       <c r="C6" s="1">
-        <f>H2*$I$54/$I$55</f>
-        <v>0.98022355975924336</v>
+        <f t="shared" ref="C6:D6" si="2">H2*$I$53/$I$54</f>
+        <v>0.97982456140350882</v>
       </c>
       <c r="D6" s="1">
-        <f>I2*$I$54/$I$55</f>
-        <v>0.98022355975924336</v>
+        <f t="shared" si="2"/>
+        <v>0.97982456140350882</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F25" si="7">F5+1</f>
+        <f t="shared" ref="F6:F25" si="3">F5+1</f>
         <v>1</v>
       </c>
       <c r="G6" s="1">
@@ -674,39 +675,39 @@
         <v>1</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:H37" si="8">G6+H$2*H5</f>
+        <f t="shared" ref="H6:H37" si="4">G6+H$2*H5</f>
         <v>4.3</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I37" si="9">H6+I$2*I5</f>
+        <f t="shared" ref="I6:I37" si="5">H6+I$2*I5</f>
         <v>7.6</v>
       </c>
       <c r="K6" s="1">
+        <f t="shared" ref="K6:M54" si="6">N6*$I6/$I$54</f>
+        <v>4.1847297750889903E-27</v>
+      </c>
+      <c r="L6" s="1">
         <f t="shared" si="1"/>
-        <v>1.2430214293237054E-27</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="2"/>
-        <v>3.1744001414915166E-2</v>
+        <v>3.2384450566268722E-2</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1744001414915166E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2384450566268722E-2</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q6)</f>
         <v>1</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="5"/>
-        <v>2.5537774865382829E+25</v>
+        <f>POWER(H$2,$Q6)</f>
+        <v>7.7387196561766152E+24</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" si="6"/>
-        <v>2.5537774865382829E+25</v>
+        <f>POWER(I$2,$Q6)</f>
+        <v>7.7387196561766152E+24</v>
       </c>
       <c r="Q6" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R6" s="1">
         <v>1</v>
@@ -718,18 +719,18 @@
       </c>
       <c r="B7" s="1">
         <f>B4*B6</f>
-        <v>29.703744235128589</v>
+        <v>29.691653375863908</v>
       </c>
       <c r="C7" s="1">
         <f>C4*C6</f>
-        <v>9.8022355975924338</v>
+        <v>9.7982456140350891</v>
       </c>
       <c r="D7" s="1">
         <f>D4*D6</f>
-        <v>9.8022355975924338</v>
+        <v>9.7982456140350891</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G7" s="1">
@@ -737,39 +738,39 @@
         <v>1</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>15.19</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>40.269999999999996</v>
       </c>
       <c r="K7" s="1">
+        <f t="shared" si="6"/>
+        <v>2.2173561584583375E-26</v>
+      </c>
+      <c r="L7" s="1">
         <f t="shared" si="1"/>
-        <v>6.586378020903371E-27</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="2"/>
-        <v>5.0970133053374556E-2</v>
+        <v>5.1998477843047904E-2</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="3"/>
-        <v>5.0970133053374556E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.1998477843047904E-2</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q7)</f>
         <v>1</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="5"/>
-        <v>7.7387196561766152E+24</v>
+        <f>POWER(H$2,$Q7)</f>
+        <v>2.3450665624777626E+24</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" si="6"/>
-        <v>7.7387196561766152E+24</v>
+        <f>POWER(I$2,$Q7)</f>
+        <v>2.3450665624777626E+24</v>
       </c>
       <c r="Q7" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R7" s="1">
         <v>2</v>
@@ -781,7 +782,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="F8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G8" s="1">
@@ -789,39 +790,39 @@
         <v>1</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>51.126999999999995</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>184.01799999999997</v>
       </c>
       <c r="K8" s="1">
+        <f t="shared" si="6"/>
+        <v>1.0132442154635866E-25</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>3.0097147023853896E-26</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="2"/>
-        <v>7.0579813111616888E-2</v>
+        <v>7.2003791797202135E-2</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="3"/>
-        <v>7.0579813111616888E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.2003791797202135E-2</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q8)</f>
         <v>1</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="5"/>
-        <v>2.3450665624777626E+24</v>
+        <f>POWER(H$2,$Q8)</f>
+        <v>7.1062623105386746E+23</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="6"/>
-        <v>2.3450665624777626E+24</v>
+        <f>POWER(I$2,$Q8)</f>
+        <v>7.1062623105386746E+23</v>
       </c>
       <c r="Q8" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R8" s="1">
         <v>3</v>
@@ -833,18 +834,18 @@
       </c>
       <c r="B9" s="1">
         <f>SUM(K6:K55)</f>
-        <v>1.4224456989046321</v>
+        <v>1.4221967963386728</v>
       </c>
       <c r="C9" s="1">
         <f>SUM(L6:L56)</f>
-        <v>25.774993570985934</v>
+        <v>25.274839932505831</v>
       </c>
       <c r="D9" s="1">
         <f>SUM(M6:M56)</f>
-        <v>25.774993570985934</v>
+        <v>25.274839932505831</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G9" s="1">
@@ -852,39 +853,39 @@
         <v>1</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>169.71909999999997</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>776.97849999999994</v>
       </c>
       <c r="K9" s="1">
+        <f t="shared" si="6"/>
+        <v>4.2782171888868177E-25</v>
+      </c>
+      <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>1.2707906916102482E-25</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="2"/>
-        <v>9.0305719963732836E-2</v>
+        <v>9.212767747177307E-2</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="3"/>
-        <v>9.0305719963732836E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.212767747177307E-2</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q9)</f>
         <v>1</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="5"/>
-        <v>7.1062623105386746E+23</v>
+        <f>POWER(H$2,$Q9)</f>
+        <v>2.153412821375356E+23</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="6"/>
-        <v>7.1062623105386746E+23</v>
+        <f>POWER(I$2,$Q9)</f>
+        <v>2.153412821375356E+23</v>
       </c>
       <c r="Q9" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R9" s="1">
         <v>4</v>
@@ -896,18 +897,18 @@
       </c>
       <c r="B10" s="1">
         <f>B9/B7</f>
-        <v>4.7887757437070938E-2</v>
+        <v>4.7898875092444816E-2</v>
       </c>
       <c r="C10" s="1">
         <f>C9/C7</f>
-        <v>2.6295015371102317</v>
+        <v>2.5795270835323763</v>
       </c>
       <c r="D10" s="1">
         <f>D9/D7</f>
-        <v>2.6295015371102317</v>
+        <v>2.5795270835323763</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G10" s="1">
@@ -915,39 +916,39 @@
         <v>1</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>561.0730299999999</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>3125.1020799999997</v>
       </c>
       <c r="K10" s="1">
+        <f t="shared" si="6"/>
+        <v>1.7207510163642812E-24</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="1"/>
-        <v>5.1112748082422171E-25</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.11006684705641655</v>
+        <v>0.11228749397071268</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="3"/>
-        <v>0.11006684705641655</v>
+        <f t="shared" si="1"/>
+        <v>0.11228749397071268</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q10)</f>
         <v>1</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="5"/>
-        <v>2.153412821375356E+23</v>
+        <f>POWER(H$2,$Q10)</f>
+        <v>6.5254933981071407E+22</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" si="6"/>
-        <v>2.153412821375356E+23</v>
+        <f>POWER(I$2,$Q10)</f>
+        <v>6.5254933981071407E+22</v>
       </c>
       <c r="Q10" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R10" s="1">
         <v>5</v>
@@ -959,18 +960,18 @@
       </c>
       <c r="B11">
         <f>B5/$B$19</f>
-        <v>9.9017027863777063</v>
+        <v>9.9057348991521383</v>
       </c>
       <c r="C11">
         <f>C5/$B$19</f>
-        <v>3.2675619195046433</v>
+        <v>3.2688925167202054</v>
       </c>
       <c r="D11">
         <f>D5/$B$19</f>
-        <v>3.2675619195046433</v>
+        <v>3.2688925167202054</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G11" s="1">
@@ -978,39 +979,39 @@
         <v>1</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>1852.5409989999996</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>12165.377862999998</v>
       </c>
       <c r="K11" s="1">
+        <f t="shared" si="6"/>
+        <v>6.6985288116453386E-24</v>
+      </c>
+      <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>1.9897138657275296E-24</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.12983864694927233</v>
+        <v>0.13245819859824889</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="3"/>
-        <v>0.12983864694927233</v>
+        <f t="shared" si="1"/>
+        <v>0.13245819859824889</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="5"/>
-        <v>6.5254933981071407E+22</v>
+        <f>POWER(H$2,$Q11)</f>
+        <v>1.977422241850649E+22</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="6"/>
-        <v>6.5254933981071407E+22</v>
+        <f>POWER(I$2,$Q11)</f>
+        <v>1.977422241850649E+22</v>
       </c>
       <c r="Q11" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R11" s="1">
         <v>6</v>
@@ -1022,18 +1023,18 @@
       </c>
       <c r="B12">
         <f>B11*B10</f>
-        <v>0.47417034124802504</v>
+        <v>0.47447355863335972</v>
       </c>
       <c r="C12">
         <f>C11*C10</f>
-        <v>8.5920590899403191</v>
+        <v>8.4321967800360813</v>
       </c>
       <c r="D12">
         <f>D11*D10</f>
-        <v>8.5920590899403191</v>
+        <v>8.4321967800360813</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G12" s="1">
@@ -1041,39 +1042,39 @@
         <v>1</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>6114.3852966999984</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>46260.13224459999</v>
       </c>
       <c r="K12" s="1">
+        <f t="shared" si="6"/>
+        <v>2.5471862210991037E-23</v>
+      </c>
+      <c r="L12" s="1">
         <f t="shared" si="1"/>
-        <v>7.5660968030771478E-24</v>
-      </c>
-      <c r="L12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.14961368102399841</v>
+        <v>0.15263220265869312</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="3"/>
-        <v>0.14961368102399841</v>
+        <f t="shared" si="1"/>
+        <v>0.15263220265869312</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q12)</f>
         <v>1</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="5"/>
-        <v>1.977422241850649E+22</v>
+        <f>POWER(H$2,$Q12)</f>
+        <v>5.9921886116686332E+21</v>
       </c>
       <c r="P12" s="1">
-        <f t="shared" si="6"/>
-        <v>1.977422241850649E+22</v>
+        <f>POWER(I$2,$Q12)</f>
+        <v>5.9921886116686332E+21</v>
       </c>
       <c r="Q12" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R12" s="1">
         <v>7</v>
@@ -1081,7 +1082,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G13" s="1">
@@ -1089,39 +1090,39 @@
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>20178.471479109994</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>172836.90788628993</v>
       </c>
       <c r="K13" s="1">
+        <f t="shared" si="6"/>
+        <v>9.5167862456061937E-23</v>
+      </c>
+      <c r="L13" s="1">
         <f t="shared" si="1"/>
-        <v>2.82684184579876E-23</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" si="2"/>
-        <v>0.16938969515383667</v>
+        <v>0.17280720654729126</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="3"/>
-        <v>0.16938969515383667</v>
+        <f t="shared" si="1"/>
+        <v>0.17280720654729126</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q13)</f>
         <v>1</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="5"/>
-        <v>5.9921886116686332E+21</v>
+        <f>POWER(H$2,$Q13)</f>
+        <v>1.8158147308086766E+21</v>
       </c>
       <c r="P13" s="1">
-        <f t="shared" si="6"/>
-        <v>5.9921886116686332E+21</v>
+        <f>POWER(I$2,$Q13)</f>
+        <v>1.8158147308086766E+21</v>
       </c>
       <c r="Q13" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R13" s="1">
         <v>8</v>
@@ -1129,7 +1130,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G14" s="1">
@@ -1137,39 +1138,39 @@
         <v>1</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>66589.955881062982</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>636951.75190581975</v>
       </c>
       <c r="K14" s="1">
+        <f t="shared" si="6"/>
+        <v>3.5071986335465523E-22</v>
+      </c>
+      <c r="L14" s="1">
         <f t="shared" si="1"/>
-        <v>1.0417693119265925E-22</v>
-      </c>
-      <c r="L14" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1891660062700726</v>
+        <v>0.19298251341411796</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="3"/>
-        <v>0.1891660062700726</v>
+        <f t="shared" si="1"/>
+        <v>0.19298251341411796</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q14)</f>
         <v>1</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="5"/>
-        <v>1.8158147308086766E+21</v>
+        <f>POWER(H$2,$Q14)</f>
+        <v>5.5024688812384145E+20</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="6"/>
-        <v>1.8158147308086766E+21</v>
+        <f>POWER(I$2,$Q14)</f>
+        <v>5.5024688812384145E+20</v>
       </c>
       <c r="Q14" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R14" s="1">
         <v>9</v>
@@ -1180,10 +1181,10 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G15" s="1">
@@ -1191,47 +1192,48 @@
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>219747.85440750784</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>2321688.6356967129</v>
       </c>
       <c r="K15" s="1">
+        <f t="shared" si="6"/>
+        <v>1.278373626616549E-21</v>
+      </c>
+      <c r="L15" s="1">
         <f t="shared" si="1"/>
-        <v>3.7972483241951737E-22</v>
-      </c>
-      <c r="L15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.20894240738218664</v>
+        <v>0.21315791209252902</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="3"/>
-        <v>0.20894240738218664</v>
+        <f t="shared" si="1"/>
+        <v>0.21315791209252902</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q15)</f>
         <v>1</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="5"/>
-        <v>5.5024688812384145E+20</v>
+        <f>POWER(H$2,$Q15)</f>
+        <v>1.6674148124964893E+20</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="6"/>
-        <v>5.5024688812384145E+20</v>
+        <f>POWER(I$2,$Q15)</f>
+        <v>1.6674148124964893E+20</v>
       </c>
       <c r="Q15" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R15" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
       <c r="F16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G16" s="1">
@@ -1239,39 +1241,39 @@
         <v>1</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>725168.91954477585</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>8386741.4173439285</v>
       </c>
       <c r="K16" s="1">
+        <f t="shared" si="6"/>
+        <v>4.6179271743593661E-21</v>
+      </c>
+      <c r="L16" s="1">
         <f t="shared" si="1"/>
-        <v>1.3716972768362066E-21</v>
-      </c>
-      <c r="L16" s="1">
-        <f t="shared" si="2"/>
-        <v>0.22871883576577884</v>
+        <v>0.23333333859263231</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="3"/>
-        <v>0.22871883576577884</v>
+        <f t="shared" si="1"/>
+        <v>0.23333333859263231</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q16)</f>
         <v>1</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="5"/>
-        <v>1.6674148124964893E+20</v>
+        <f>POWER(H$2,$Q16)</f>
+        <v>5.0527721590802711E+19</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" si="6"/>
-        <v>1.6674148124964893E+20</v>
+        <f>POWER(I$2,$Q16)</f>
+        <v>5.0527721590802711E+19</v>
       </c>
       <c r="Q16" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R16" s="1">
         <v>11</v>
@@ -1279,7 +1281,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G17" s="1">
@@ -1287,39 +1289,39 @@
         <v>1</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>2393058.4344977601</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>30069305.111732721</v>
       </c>
       <c r="K17" s="1">
+        <f t="shared" si="6"/>
+        <v>1.6556831107539937E-20</v>
+      </c>
+      <c r="L17" s="1">
         <f t="shared" si="1"/>
-        <v>4.9179987656258705E-21</v>
-      </c>
-      <c r="L17" s="1">
-        <f t="shared" si="2"/>
-        <v>0.24849527241345537</v>
+        <v>0.25350877352355139</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="3"/>
-        <v>0.24849527241345537</v>
+        <f t="shared" si="1"/>
+        <v>0.25350877352355139</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q17)</f>
         <v>1</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="5"/>
-        <v>5.0527721590802711E+19</v>
+        <f>POWER(H$2,$Q17)</f>
+        <v>1.5311430785091729E+19</v>
       </c>
       <c r="P17" s="1">
-        <f t="shared" si="6"/>
-        <v>5.0527721590802711E+19</v>
+        <f>POWER(I$2,$Q17)</f>
+        <v>1.5311430785091729E+19</v>
       </c>
       <c r="Q17" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R17" s="1">
         <v>12</v>
@@ -1333,7 +1335,7 @@
         <v>0.34</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="G18" s="1">
@@ -1341,39 +1343,39 @@
         <v>1</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>7897093.8338426081</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>107125800.70256057</v>
       </c>
       <c r="K18" s="1">
+        <f t="shared" si="6"/>
+        <v>5.8985858931612423E-20</v>
+      </c>
+      <c r="L18" s="1">
         <f t="shared" si="1"/>
-        <v>1.7521008671939903E-20</v>
-      </c>
-      <c r="L18" s="1">
-        <f t="shared" si="2"/>
-        <v>0.26827171156539975</v>
+        <v>0.27368421100926316</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="3"/>
-        <v>0.26827171156539975</v>
+        <f t="shared" si="1"/>
+        <v>0.27368421100926316</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q18)</f>
         <v>1</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="5"/>
-        <v>1.5311430785091729E+19</v>
+        <f>POWER(H$2,$Q18)</f>
+        <v>4.639827510633858E+18</v>
       </c>
       <c r="P18" s="1">
-        <f t="shared" si="6"/>
-        <v>1.5311430785091729E+19</v>
+        <f>POWER(I$2,$Q18)</f>
+        <v>4.639827510633858E+18</v>
       </c>
       <c r="Q18" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R18" s="1">
         <v>13</v>
@@ -1385,10 +1387,10 @@
       </c>
       <c r="B19">
         <f>B18*B7</f>
-        <v>10.099273039943721</v>
+        <v>10.095162147793729</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="G19" s="1">
@@ -1396,39 +1398,39 @@
         <v>1</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>26060410.651680604</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>379575552.97013044</v>
       </c>
       <c r="K19" s="1">
+        <f t="shared" si="6"/>
+        <v>2.0900277873815437E-19</v>
+      </c>
+      <c r="L19" s="1">
         <f t="shared" si="1"/>
-        <v>6.2081650840693086E-20</v>
-      </c>
-      <c r="L19" s="1">
-        <f t="shared" si="2"/>
-        <v>0.28804815147621338</v>
+        <v>0.29385964926915453</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="3"/>
-        <v>0.28804815147621338</v>
+        <f t="shared" si="1"/>
+        <v>0.29385964926915453</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q19)</f>
         <v>1</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="5"/>
-        <v>4.639827510633858E+18</v>
+        <f>POWER(H$2,$Q19)</f>
+        <v>1.4060083365557148E+18</v>
       </c>
       <c r="P19" s="1">
-        <f t="shared" si="6"/>
-        <v>4.639827510633858E+18</v>
+        <f>POWER(I$2,$Q19)</f>
+        <v>1.4060083365557148E+18</v>
       </c>
       <c r="Q19" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R19" s="1">
         <v>14</v>
@@ -1440,10 +1442,10 @@
       </c>
       <c r="B20">
         <f>B15/B19</f>
-        <v>4.9508513931888531</v>
+        <v>4.853810100584548</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="G20" s="1">
@@ -1451,39 +1453,39 @@
         <v>1</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>85999356.150545985</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1338598680.9519765</v>
       </c>
       <c r="K20" s="1">
+        <f t="shared" si="6"/>
+        <v>7.3706233645718214E-19</v>
+      </c>
+      <c r="L20" s="1">
         <f t="shared" si="1"/>
-        <v>2.1893511127470434E-19</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" si="2"/>
-        <v>0.30782459161698733</v>
+        <v>0.3140350877636458</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="3"/>
-        <v>0.30782459161698733</v>
+        <f t="shared" si="1"/>
+        <v>0.3140350877636458</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q20)</f>
         <v>1</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="5"/>
-        <v>1.4060083365557148E+18</v>
+        <f>POWER(H$2,$Q20)</f>
+        <v>4.260631322896105E+17</v>
       </c>
       <c r="P20" s="1">
-        <f t="shared" si="6"/>
-        <v>1.4060083365557148E+18</v>
+        <f>POWER(I$2,$Q20)</f>
+        <v>4.260631322896105E+17</v>
       </c>
       <c r="Q20" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R20" s="1">
         <v>15</v>
@@ -1491,7 +1493,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G21" s="1">
@@ -1499,39 +1501,39 @@
         <v>1</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>283797876.29680175</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>4701173523.438324</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="1"/>
-        <v>7.689025569214561E-19</v>
+        <f t="shared" si="6"/>
+        <v>2.5885711607095233E-18</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="2"/>
-        <v>0.3276010318274461</v>
+        <f t="shared" si="6"/>
+        <v>0.33421052632922793</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="3"/>
-        <v>0.3276010318274461</v>
+        <f t="shared" si="6"/>
+        <v>0.33421052632922793</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q21)</f>
         <v>1</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="5"/>
-        <v>4.260631322896105E+17</v>
+        <f>POWER(H$2,$Q21)</f>
+        <v>1.2911004008776077E+17</v>
       </c>
       <c r="P21" s="1">
-        <f t="shared" si="6"/>
-        <v>4.260631322896105E+17</v>
+        <f>POWER(I$2,$Q21)</f>
+        <v>1.2911004008776077E+17</v>
       </c>
       <c r="Q21" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R21" s="1">
         <v>16</v>
@@ -1539,7 +1541,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="G22" s="1">
@@ -1547,39 +1549,39 @@
         <v>1</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>936532992.77944577</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>16450405620.125914</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="1"/>
-        <v>2.6905535140636359E-18</v>
+        <f t="shared" si="6"/>
+        <v>9.0579608172147619E-18</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="2"/>
-        <v>0.34737747205902159</v>
+        <f t="shared" si="6"/>
+        <v>0.35438596491635282</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="3"/>
-        <v>0.34737747205902159</v>
+        <f t="shared" si="6"/>
+        <v>0.35438596491635282</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q22)</f>
         <v>1</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="5"/>
-        <v>1.2911004008776077E+17</v>
+        <f>POWER(H$2,$Q22)</f>
+        <v>3.912425457204872E+16</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" si="6"/>
-        <v>1.2911004008776077E+17</v>
+        <f>POWER(I$2,$Q22)</f>
+        <v>3.912425457204872E+16</v>
       </c>
       <c r="Q22" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R22" s="1">
         <v>17</v>
@@ -1587,7 +1589,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G23" s="1">
@@ -1595,39 +1597,39 @@
         <v>1</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>3090558877.1721706</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>57376897423.587685</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="1"/>
-        <v>9.3843043481088944E-18</v>
+        <f t="shared" si="6"/>
+        <v>3.1593001454041339E-17</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="2"/>
-        <v>0.36715391229699612</v>
+        <f t="shared" si="6"/>
+        <v>0.37456140351000583</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="3"/>
-        <v>0.36715391229699612</v>
+        <f t="shared" si="6"/>
+        <v>0.37456140351000583</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q23)</f>
         <v>1</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="5"/>
-        <v>3.912425457204872E+16</v>
+        <f>POWER(H$2,$Q23)</f>
+        <v>1.1855834718802646E+16</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" si="6"/>
-        <v>3.912425457204872E+16</v>
+        <f>POWER(I$2,$Q23)</f>
+        <v>1.1855834718802646E+16</v>
       </c>
       <c r="Q23" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R23" s="1">
         <v>18</v>
@@ -1635,7 +1637,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="G24" s="1">
@@ -1643,39 +1645,39 @@
         <v>1</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>10198844295.668163</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>199542605793.50751</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="1"/>
-        <v>3.2636280929529266E-17</v>
+        <f t="shared" si="6"/>
+        <v>1.0987261629775471E-16</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="2"/>
-        <v>0.38693035253690983</v>
+        <f t="shared" si="6"/>
+        <v>0.39473684210563686</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="3"/>
-        <v>0.38693035253690983</v>
+        <f t="shared" si="6"/>
+        <v>0.39473684210563686</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q24)</f>
         <v>1</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="5"/>
-        <v>1.1855834718802646E+16</v>
+        <f>POWER(H$2,$Q24)</f>
+        <v>3592677187515953</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1855834718802646E+16</v>
+        <f>POWER(I$2,$Q24)</f>
+        <v>3592677187515953</v>
       </c>
       <c r="Q24" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R24" s="1">
         <v>19</v>
@@ -1683,7 +1685,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G25" s="1">
@@ -1691,39 +1693,39 @@
         <v>1</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>33656186176.704937</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>692146785295.27966</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1320437978415086E-16</v>
+        <f t="shared" si="6"/>
+        <v>3.8111148173122154E-16</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="2"/>
-        <v>0.4067067927774109</v>
+        <f t="shared" si="6"/>
+        <v>0.41491228070186753</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="3"/>
-        <v>0.4067067927774109</v>
+        <f t="shared" si="6"/>
+        <v>0.41491228070186753</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q25)</f>
         <v>1</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="5"/>
-        <v>3592677187515953</v>
+        <f>POWER(H$2,$Q25)</f>
+        <v>1088690056823016.3</v>
       </c>
       <c r="P25" s="1">
-        <f t="shared" si="6"/>
-        <v>3592677187515953</v>
+        <f>POWER(I$2,$Q25)</f>
+        <v>1088690056823016.3</v>
       </c>
       <c r="Q25" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R25" s="1">
         <v>20</v>
@@ -1738,39 +1740,39 @@
         <v>1</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>111065414384.12628</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>2395149805858.5493</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="1"/>
-        <v>3.9173980725298553E-16</v>
+        <f t="shared" si="6"/>
+        <v>1.3188229879440641E-15</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="2"/>
-        <v>0.42648323301809027</v>
+        <f t="shared" si="6"/>
+        <v>0.43508771929827977</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="3"/>
-        <v>0.42648323301809027</v>
+        <f t="shared" si="6"/>
+        <v>0.43508771929827977</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q26)</f>
         <v>1</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="5"/>
-        <v>1088690056823016.3</v>
+        <f>POWER(H$2,$Q26)</f>
+        <v>329906077825156.44</v>
       </c>
       <c r="P26" s="1">
-        <f t="shared" si="6"/>
-        <v>1088690056823016.3</v>
+        <f>POWER(I$2,$Q26)</f>
+        <v>329906077825156.44</v>
       </c>
       <c r="Q26" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R26" s="1">
         <v>21</v>
@@ -1785,39 +1787,39 @@
         <v>1</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>366515867468.6167</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>8270510226801.8281</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="1"/>
-        <v>1.3526870320204649E-15</v>
+        <f t="shared" si="6"/>
+        <v>4.5539276843783704E-15</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="2"/>
-        <v>0.44625967325882337</v>
+        <f t="shared" si="6"/>
+        <v>0.45526315789474708</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="3"/>
-        <v>0.44625967325882337</v>
+        <f t="shared" si="6"/>
+        <v>0.45526315789474708</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q27)</f>
         <v>1</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="5"/>
-        <v>329906077825156.44</v>
+        <f>POWER(H$2,$Q27)</f>
+        <v>99971538734895.906</v>
       </c>
       <c r="P27" s="1">
-        <f t="shared" si="6"/>
-        <v>329906077825156.44</v>
+        <f>POWER(I$2,$Q27)</f>
+        <v>99971538734895.906</v>
       </c>
       <c r="Q27" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R27" s="1">
         <v>22</v>
@@ -1832,39 +1834,39 @@
         <v>1</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>1209502362647.4351</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>28502186111093.465</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="1"/>
-        <v>4.6616879103502193E-15</v>
+        <f t="shared" si="6"/>
+        <v>1.5693940378186937E-14</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="2"/>
-        <v>0.46603611349957286</v>
+        <f t="shared" si="6"/>
+        <v>0.47543859649123094</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="3"/>
-        <v>0.46603611349957286</v>
+        <f t="shared" si="6"/>
+        <v>0.47543859649123094</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q28)</f>
         <v>1</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="5"/>
-        <v>99971538734895.906</v>
+        <f>POWER(H$2,$Q28)</f>
+        <v>30294405677241.184</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" si="6"/>
-        <v>99971538734895.906</v>
+        <f>POWER(I$2,$Q28)</f>
+        <v>30294405677241.184</v>
       </c>
       <c r="Q28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R28" s="1">
         <v>23</v>
@@ -1879,39 +1881,39 @@
         <v>1</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>3991357796737.5356</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>98048571963345.953</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6036378429608748E-14</v>
+        <f t="shared" si="6"/>
+        <v>5.3987734013153874E-14</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="2"/>
-        <v>0.48581255374032734</v>
+        <f t="shared" si="6"/>
+        <v>0.4956140350877199</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="3"/>
-        <v>0.48581255374032734</v>
+        <f t="shared" si="6"/>
+        <v>0.4956140350877199</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q29)</f>
         <v>1</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="5"/>
-        <v>30294405677241.184</v>
+        <f>POWER(H$2,$Q29)</f>
+        <v>9180122932497.3281</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" si="6"/>
-        <v>30294405677241.184</v>
+        <f>POWER(I$2,$Q29)</f>
+        <v>9180122932497.3281</v>
       </c>
       <c r="Q29" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R29" s="1">
         <v>24</v>
@@ -1926,39 +1928,39 @@
         <v>1</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>13171480729234.867</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>336731768208276.5</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="1"/>
-        <v>5.5074316291704025E-14</v>
+        <f t="shared" si="6"/>
+        <v>1.8541203376836041E-13</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="2"/>
-        <v>0.50558899398108326</v>
+        <f t="shared" si="6"/>
+        <v>0.51578947368421046</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="3"/>
-        <v>0.50558899398108326</v>
+        <f t="shared" si="6"/>
+        <v>0.51578947368421046</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q30)</f>
         <v>1</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="5"/>
-        <v>9180122932497.3281</v>
+        <f>POWER(H$2,$Q30)</f>
+        <v>2781855434090.0996</v>
       </c>
       <c r="P30" s="1">
-        <f t="shared" si="6"/>
-        <v>9180122932497.3281</v>
+        <f>POWER(I$2,$Q30)</f>
+        <v>2781855434090.0996</v>
       </c>
       <c r="Q30" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R30" s="1">
         <v>25</v>
@@ -1973,39 +1975,39 @@
         <v>1</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>43465886406476.063</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1154680721493788.5</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8885432642680744E-13</v>
+        <f t="shared" si="6"/>
+        <v>6.3579299946793362E-13</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="2"/>
-        <v>0.52536543422183979</v>
+        <f t="shared" si="6"/>
+        <v>0.53596491228070153</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="3"/>
-        <v>0.52536543422183979</v>
+        <f t="shared" si="6"/>
+        <v>0.53596491228070153</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q31)</f>
         <v>1</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="5"/>
-        <v>2781855434090.0996</v>
+        <f>POWER(H$2,$Q31)</f>
+        <v>842986495178.81812</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" si="6"/>
-        <v>2781855434090.0996</v>
+        <f>POWER(I$2,$Q31)</f>
+        <v>842986495178.81812</v>
       </c>
       <c r="Q31" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R31" s="1">
         <v>26</v>
@@ -2020,39 +2022,39 @@
         <v>1</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>143437425141372</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>3953883806070874</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="1"/>
-        <v>6.4667925000027253E-13</v>
+        <f t="shared" si="6"/>
+        <v>2.1770967487509175E-12</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="2"/>
-        <v>0.54514187446259632</v>
+        <f t="shared" si="6"/>
+        <v>0.55614035087719271</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="3"/>
-        <v>0.54514187446259632</v>
+        <f t="shared" si="6"/>
+        <v>0.55614035087719271</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q32)</f>
         <v>1</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="5"/>
-        <v>842986495178.81812</v>
+        <f>POWER(H$2,$Q32)</f>
+        <v>255450453084.49036</v>
       </c>
       <c r="P32" s="1">
-        <f t="shared" si="6"/>
-        <v>842986495178.81812</v>
+        <f>POWER(I$2,$Q32)</f>
+        <v>255450453084.49036</v>
       </c>
       <c r="Q32" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R32" s="1">
         <v>27</v>
@@ -2067,39 +2069,39 @@
         <v>1</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>473343502966528.56</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1.3521160063000412E+16</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="1"/>
-        <v>2.2114594352138655E-12</v>
+        <f t="shared" si="6"/>
+        <v>7.4450527775502581E-12</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="2"/>
-        <v>0.56491831470335307</v>
+        <f t="shared" si="6"/>
+        <v>0.57631578947368389</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="3"/>
-        <v>0.56491831470335307</v>
+        <f t="shared" si="6"/>
+        <v>0.57631578947368389</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q33)</f>
         <v>1</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="5"/>
-        <v>255450453084.49036</v>
+        <f>POWER(H$2,$Q33)</f>
+        <v>77409228207.421326</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="6"/>
-        <v>255450453084.49036</v>
+        <f>POWER(I$2,$Q33)</f>
+        <v>77409228207.421326</v>
       </c>
       <c r="Q33" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R33" s="1">
         <v>28</v>
@@ -2114,39 +2116,39 @@
         <v>1</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>1562033559789545.3</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>4.6181861767690904E+16</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="1"/>
-        <v>7.553295239908545E-12</v>
+        <f t="shared" si="6"/>
+        <v>2.5428764737934213E-11</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="2"/>
-        <v>0.58469475494410972</v>
+        <f t="shared" si="6"/>
+        <v>0.59649122807017507</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="3"/>
-        <v>0.58469475494410972</v>
+        <f t="shared" si="6"/>
+        <v>0.59649122807017507</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q34)</f>
         <v>1</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="5"/>
-        <v>77409228207.421326</v>
+        <f>POWER(H$2,$Q34)</f>
+        <v>23457341881.036766</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" si="6"/>
-        <v>77409228207.421326</v>
+        <f>POWER(I$2,$Q34)</f>
+        <v>23457341881.036766</v>
       </c>
       <c r="Q34" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R34" s="1">
         <v>29</v>
@@ -2161,39 +2163,39 @@
         <v>1</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>5154710747305500</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1.5755485458068547E+17</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="1"/>
-        <v>2.57689553339174E-11</v>
+        <f t="shared" si="6"/>
+        <v>8.6753222522843491E-11</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60447119518486636</v>
+        <f t="shared" si="6"/>
+        <v>0.61666666666666636</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="3"/>
-        <v>0.60447119518486636</v>
+        <f t="shared" si="6"/>
+        <v>0.61666666666666636</v>
       </c>
       <c r="N35" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q35)</f>
         <v>1</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="5"/>
-        <v>23457341881.036766</v>
+        <f>POWER(H$2,$Q35)</f>
+        <v>7108285418.4959908</v>
       </c>
       <c r="P35" s="1">
-        <f t="shared" si="6"/>
-        <v>23457341881.036766</v>
+        <f>POWER(I$2,$Q35)</f>
+        <v>7108285418.4959908</v>
       </c>
       <c r="Q35" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R35" s="1">
         <v>30</v>
@@ -2208,39 +2210,39 @@
         <v>1</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>1.7010545466108152E+16</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>5.3694156558237018E+17</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="1"/>
-        <v>8.781972004125078E-11</v>
+        <f t="shared" si="6"/>
+        <v>2.9565202065466347E-10</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="2"/>
-        <v>0.62424763542562312</v>
+        <f t="shared" si="6"/>
+        <v>0.63684210526315765</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="3"/>
-        <v>0.62424763542562312</v>
+        <f t="shared" si="6"/>
+        <v>0.63684210526315765</v>
       </c>
       <c r="N36" s="1">
-        <f t="shared" si="4"/>
+        <f>POWER(G$2,$Q36)</f>
         <v>1</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="5"/>
-        <v>7108285418.4959908</v>
+        <f>POWER(H$2,$Q36)</f>
+        <v>2154025884.3927245</v>
       </c>
       <c r="P36" s="1">
-        <f t="shared" si="6"/>
-        <v>7108285418.4959908</v>
+        <f>POWER(I$2,$Q36)</f>
+        <v>2154025884.3927245</v>
       </c>
       <c r="Q36" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R36" s="1">
         <v>31</v>
@@ -2251,43 +2253,43 @@
         <v>32</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" ref="G37:G55" si="10">POWER(G$2,R37)</f>
+        <f t="shared" ref="G37:G55" si="7">POWER(G$2,R37)</f>
         <v>1</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>5.6134800038156896E+16</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1.8280419664599782E+18</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" ref="K37:K55" si="11">N37*$I37/$I$55</f>
-        <v>2.9898622868589469E-10</v>
+        <f t="shared" si="6"/>
+        <v>1.0065607430470133E-9</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" ref="L37:L55" si="12">O37*$I37/$I$55</f>
-        <v>0.64402407566637965</v>
+        <f t="shared" si="6"/>
+        <v>0.65701754385964861</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" ref="M37:M55" si="13">P37*$I37/$I$55</f>
-        <v>0.64402407566637965</v>
+        <f t="shared" si="6"/>
+        <v>0.65701754385964861</v>
       </c>
       <c r="N37" s="1">
-        <f t="shared" ref="N37:N55" si="14">POWER(G$2,$Q37)</f>
+        <f>POWER(G$2,$Q37)</f>
         <v>1</v>
       </c>
       <c r="O37" s="1">
-        <f t="shared" ref="O37:O55" si="15">POWER(H$2,$Q37)</f>
-        <v>2154025884.3927245</v>
+        <f>POWER(H$2,$Q37)</f>
+        <v>652735116.48264372</v>
       </c>
       <c r="P37" s="1">
-        <f t="shared" ref="P37:P55" si="16">POWER(I$2,$Q37)</f>
-        <v>2154025884.3927245</v>
+        <f>POWER(I$2,$Q37)</f>
+        <v>652735116.48264372</v>
       </c>
       <c r="Q37" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R37" s="1">
         <v>32</v>
@@ -2298,43 +2300,43 @@
         <v>33</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" ref="H38:H69" si="17">G38+H$2*H37</f>
+        <f t="shared" ref="H38:H55" si="8">G38+H$2*H37</f>
         <v>1.8524484012591776E+17</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" ref="I38:I69" si="18">H38+I$2*I37</f>
+        <f t="shared" ref="I38:I55" si="9">H38+I$2*I37</f>
         <v>6.2177833294438461E+18</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="11"/>
-        <v>1.016952358077684E-9</v>
+        <f t="shared" si="6"/>
+        <v>3.4236503991810031E-9</v>
       </c>
       <c r="L38" s="1">
-        <f t="shared" si="12"/>
-        <v>0.66380051590713629</v>
+        <f t="shared" si="6"/>
+        <v>0.67719298245614001</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="13"/>
-        <v>0.66380051590713629</v>
+        <f t="shared" si="6"/>
+        <v>0.67719298245614001</v>
       </c>
       <c r="N38" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q38)</f>
         <v>1</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="15"/>
-        <v>652735116.48264372</v>
+        <f>POWER(H$2,$Q38)</f>
+        <v>197798520.1462557</v>
       </c>
       <c r="P38" s="1">
-        <f t="shared" si="16"/>
-        <v>652735116.48264372</v>
+        <f>POWER(I$2,$Q38)</f>
+        <v>197798520.1462557</v>
       </c>
       <c r="Q38" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R38" s="1">
         <v>33</v>
@@ -2345,43 +2347,43 @@
         <v>34</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>6.1130797241552858E+17</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>2.1129992959580221E+19</v>
       </c>
       <c r="K39" s="1">
-        <f t="shared" si="11"/>
-        <v>3.4559255329233214E-9</v>
+        <f t="shared" si="6"/>
+        <v>1.1634646142812644E-8</v>
       </c>
       <c r="L39" s="1">
-        <f t="shared" si="12"/>
-        <v>0.68357695614789304</v>
+        <f t="shared" si="6"/>
+        <v>0.69736842105263142</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="13"/>
-        <v>0.68357695614789304</v>
+        <f t="shared" si="6"/>
+        <v>0.69736842105263142</v>
       </c>
       <c r="N39" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q39)</f>
         <v>1</v>
       </c>
       <c r="O39" s="1">
-        <f t="shared" si="15"/>
-        <v>197798520.1462557</v>
+        <f>POWER(H$2,$Q39)</f>
+        <v>59938945.498865373</v>
       </c>
       <c r="P39" s="1">
-        <f t="shared" si="16"/>
-        <v>197798520.1462557</v>
+        <f>POWER(I$2,$Q39)</f>
+        <v>59938945.498865373</v>
       </c>
       <c r="Q39" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R39" s="1">
         <v>34</v>
@@ -2392,43 +2394,43 @@
         <v>35</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>2.0173163089712443E+18</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>7.1746293075585966E+19</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="11"/>
-        <v>1.173449733782794E-8</v>
+        <f t="shared" si="6"/>
+        <v>3.950511169548233E-8</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" si="12"/>
-        <v>0.7033533963886498</v>
+        <f t="shared" si="6"/>
+        <v>0.71754385964912237</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="13"/>
-        <v>0.7033533963886498</v>
+        <f t="shared" si="6"/>
+        <v>0.71754385964912237</v>
       </c>
       <c r="N40" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q40)</f>
         <v>1</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="15"/>
-        <v>59938945.498865373</v>
+        <f>POWER(H$2,$Q40)</f>
+        <v>18163316.817837991</v>
       </c>
       <c r="P40" s="1">
-        <f t="shared" si="16"/>
-        <v>59938945.498865373</v>
+        <f>POWER(I$2,$Q40)</f>
+        <v>18163316.817837991</v>
       </c>
       <c r="Q40" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R40" s="1">
         <v>35</v>
@@ -2439,43 +2441,43 @@
         <v>36</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>6.6571438196051057E+18</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>2.434199109690388E+20</v>
       </c>
       <c r="K41" s="1">
-        <f t="shared" si="11"/>
-        <v>3.981265337612944E-8</v>
+        <f t="shared" si="6"/>
+        <v>1.3403244069495366E-7</v>
       </c>
       <c r="L41" s="1">
-        <f t="shared" si="12"/>
-        <v>0.72312983662940633</v>
+        <f t="shared" si="6"/>
+        <v>0.73771929824561377</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="13"/>
-        <v>0.72312983662940633</v>
+        <f t="shared" si="6"/>
+        <v>0.73771929824561377</v>
       </c>
       <c r="N41" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q41)</f>
         <v>1</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="15"/>
-        <v>18163316.817837991</v>
+        <f>POWER(H$2,$Q41)</f>
+        <v>5504035.3993448466</v>
       </c>
       <c r="P41" s="1">
-        <f t="shared" si="16"/>
-        <v>18163316.817837991</v>
+        <f>POWER(I$2,$Q41)</f>
+        <v>5504035.3993448466</v>
       </c>
       <c r="Q41" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R41" s="1">
         <v>36</v>
@@ -2486,43 +2488,43 @@
         <v>37</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>2.1968574604696846E+19</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>8.2525428080252486E+20</v>
       </c>
       <c r="K42" s="1">
-        <f t="shared" si="11"/>
-        <v>1.3497483627350804E-7</v>
+        <f t="shared" si="6"/>
+        <v>4.5440344222289168E-7</v>
       </c>
       <c r="L42" s="1">
-        <f t="shared" si="12"/>
-        <v>0.74290627687016308</v>
+        <f t="shared" si="6"/>
+        <v>0.75789473684210507</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="13"/>
-        <v>0.74290627687016308</v>
+        <f t="shared" si="6"/>
+        <v>0.75789473684210507</v>
       </c>
       <c r="N42" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q42)</f>
         <v>1</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="15"/>
-        <v>5504035.3993448466</v>
+        <f>POWER(H$2,$Q42)</f>
+        <v>1667889.5149529839</v>
       </c>
       <c r="P42" s="1">
-        <f t="shared" si="16"/>
-        <v>5504035.3993448466</v>
+        <f>POWER(I$2,$Q42)</f>
+        <v>1667889.5149529839</v>
       </c>
       <c r="Q42" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R42" s="1">
         <v>37</v>
@@ -2533,43 +2535,43 @@
         <v>38</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>7.249629619549959E+19</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>2.7958354228438316E+21</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" si="11"/>
-        <v>4.5727412413910345E-7</v>
+        <f t="shared" si="6"/>
+        <v>1.5394494395030396E-6</v>
       </c>
       <c r="L43" s="1">
-        <f t="shared" si="12"/>
-        <v>0.76268271711091984</v>
+        <f t="shared" si="6"/>
+        <v>0.77807017543859636</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="13"/>
-        <v>0.76268271711091984</v>
+        <f t="shared" si="6"/>
+        <v>0.77807017543859636</v>
       </c>
       <c r="N43" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q43)</f>
         <v>1</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="15"/>
-        <v>1667889.5149529839</v>
+        <f>POWER(H$2,$Q43)</f>
+        <v>505421.06513726793</v>
       </c>
       <c r="P43" s="1">
-        <f t="shared" si="16"/>
-        <v>1667889.5149529839</v>
+        <f>POWER(I$2,$Q43)</f>
+        <v>505421.06513726793</v>
       </c>
       <c r="Q43" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R43" s="1">
         <v>38</v>
@@ -2580,43 +2582,43 @@
         <v>39</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>2.3923777744514862E+20</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>9.4654946728297932E+21</v>
       </c>
       <c r="K44" s="1">
-        <f t="shared" si="11"/>
-        <v>1.5481332522995803E-6</v>
+        <f t="shared" si="6"/>
+        <v>5.2119128149127713E-6</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" si="12"/>
-        <v>0.7824591573516767</v>
+        <f t="shared" si="6"/>
+        <v>0.79824561403508765</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="13"/>
-        <v>0.7824591573516767</v>
+        <f t="shared" si="6"/>
+        <v>0.79824561403508765</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q44)</f>
         <v>1</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="15"/>
-        <v>505421.06513726793</v>
+        <f>POWER(H$2,$Q44)</f>
+        <v>153157.89852644483</v>
       </c>
       <c r="P44" s="1">
-        <f t="shared" si="16"/>
-        <v>505421.06513726793</v>
+        <f>POWER(I$2,$Q44)</f>
+        <v>153157.89852644483</v>
       </c>
       <c r="Q44" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R44" s="1">
         <v>39</v>
@@ -2627,43 +2629,43 @@
         <v>40</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>7.8948466556899046E+20</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>3.2025617085907308E+22</v>
       </c>
       <c r="K45" s="1">
-        <f t="shared" si="11"/>
-        <v>5.2379642533023928E-6</v>
+        <f t="shared" si="6"/>
+        <v>1.763402018223619E-5</v>
       </c>
       <c r="L45" s="1">
-        <f t="shared" si="12"/>
-        <v>0.80223559759243324</v>
+        <f t="shared" si="6"/>
+        <v>0.81842105263157883</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="13"/>
-        <v>0.80223559759243324</v>
+        <f t="shared" si="6"/>
+        <v>0.81842105263157883</v>
       </c>
       <c r="N45" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q45)</f>
         <v>1</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="15"/>
-        <v>153157.89852644483</v>
+        <f>POWER(H$2,$Q45)</f>
+        <v>46411.484401952977</v>
       </c>
       <c r="P45" s="1">
-        <f t="shared" si="16"/>
-        <v>153157.89852644483</v>
+        <f>POWER(I$2,$Q45)</f>
+        <v>46411.484401952977</v>
       </c>
       <c r="Q45" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R45" s="1">
         <v>40</v>
@@ -2674,43 +2676,43 @@
         <v>41</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H46" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>2.6052993963776682E+21</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>1.0828983577987179E+23</v>
       </c>
       <c r="K46" s="1">
-        <f t="shared" si="11"/>
-        <v>1.7711392954253365E-5</v>
+        <f t="shared" si="6"/>
+        <v>5.9626802648358769E-5</v>
       </c>
       <c r="L46" s="1">
-        <f t="shared" si="12"/>
-        <v>0.82201203783318999</v>
+        <f t="shared" si="6"/>
+        <v>0.83859649122807023</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="13"/>
-        <v>0.82201203783318999</v>
+        <f t="shared" si="6"/>
+        <v>0.83859649122807023</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q46)</f>
         <v>1</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="15"/>
-        <v>46411.484401952977</v>
+        <f>POWER(H$2,$Q46)</f>
+        <v>14064.086182409994</v>
       </c>
       <c r="P46" s="1">
-        <f t="shared" si="16"/>
-        <v>46411.484401952977</v>
+        <f>POWER(I$2,$Q46)</f>
+        <v>14064.086182409994</v>
       </c>
       <c r="Q46" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R46" s="1">
         <v>41</v>
@@ -2721,43 +2723,43 @@
         <v>42</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>8.5974880080463051E+21</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>3.6595394608162319E+23</v>
       </c>
       <c r="K47" s="1">
-        <f t="shared" si="11"/>
-        <v>5.9853762779609147E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.0150241769461576E-4</v>
       </c>
       <c r="L47" s="1">
-        <f t="shared" si="12"/>
-        <v>0.84178847807394674</v>
+        <f t="shared" si="6"/>
+        <v>0.85877192982456141</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="13"/>
-        <v>0.84178847807394674</v>
+        <f t="shared" si="6"/>
+        <v>0.85877192982456141</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q47)</f>
         <v>1</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="15"/>
-        <v>14064.086182409994</v>
+        <f>POWER(H$2,$Q47)</f>
+        <v>4261.8442976999986</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" si="16"/>
-        <v>14064.086182409994</v>
+        <f>POWER(I$2,$Q47)</f>
+        <v>4261.8442976999986</v>
       </c>
       <c r="Q47" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R47" s="1">
         <v>42</v>
@@ -2768,43 +2770,43 @@
         <v>43</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>2.8371710426552807E+22</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>1.2360197324959093E+24</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" si="11"/>
-        <v>2.0215776507360122E-4</v>
+        <f t="shared" si="6"/>
+        <v>6.8058007594383701E-4</v>
       </c>
       <c r="L48" s="1">
-        <f t="shared" si="12"/>
-        <v>0.86156491831470339</v>
+        <f t="shared" si="6"/>
+        <v>0.87894736842105259</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="13"/>
-        <v>0.86156491831470339</v>
+        <f t="shared" si="6"/>
+        <v>0.87894736842105259</v>
       </c>
       <c r="N48" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q48)</f>
         <v>1</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="15"/>
-        <v>4261.8442976999986</v>
+        <f>POWER(H$2,$Q48)</f>
+        <v>1291.4679689999996</v>
       </c>
       <c r="P48" s="1">
-        <f t="shared" si="16"/>
-        <v>4261.8442976999986</v>
+        <f>POWER(I$2,$Q48)</f>
+        <v>1291.4679689999996</v>
       </c>
       <c r="Q48" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R48" s="1">
         <v>43</v>
@@ -2815,43 +2817,43 @@
         <v>44</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>9.3626644407624256E+22</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>4.1724917616441245E+24</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="11"/>
-        <v>6.8243377281582444E-4</v>
+        <f t="shared" si="6"/>
+        <v>2.2974671725349586E-3</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" si="12"/>
-        <v>0.88134135855545992</v>
+        <f t="shared" si="6"/>
+        <v>0.89912280701754388</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="13"/>
-        <v>0.88134135855545992</v>
+        <f t="shared" si="6"/>
+        <v>0.89912280701754388</v>
       </c>
       <c r="N49" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q49)</f>
         <v>1</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="15"/>
-        <v>1291.4679689999996</v>
+        <f>POWER(H$2,$Q49)</f>
+        <v>391.35392999999988</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" si="16"/>
-        <v>1291.4679689999996</v>
+        <f>POWER(I$2,$Q49)</f>
+        <v>391.35392999999988</v>
       </c>
       <c r="Q49" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R49" s="1">
         <v>44</v>
@@ -2862,43 +2864,43 @@
         <v>45</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>3.0896792654516004E+23</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>1.407819073997077E+25</v>
       </c>
       <c r="K50" s="1">
-        <f t="shared" si="11"/>
-        <v>2.302564838932924E-3</v>
+        <f t="shared" si="6"/>
+        <v>7.7517663117023412E-3</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" si="12"/>
-        <v>0.90111779879621656</v>
+        <f t="shared" si="6"/>
+        <v>0.91929824561403506</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="13"/>
-        <v>0.90111779879621656</v>
+        <f t="shared" si="6"/>
+        <v>0.91929824561403506</v>
       </c>
       <c r="N50" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q50)</f>
         <v>1</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="15"/>
-        <v>391.35392999999988</v>
+        <f>POWER(H$2,$Q50)</f>
+        <v>118.59209999999997</v>
       </c>
       <c r="P50" s="1">
-        <f t="shared" si="16"/>
-        <v>391.35392999999988</v>
+        <f>POWER(I$2,$Q50)</f>
+        <v>118.59209999999997</v>
       </c>
       <c r="Q50" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R50" s="1">
         <v>45</v>
@@ -2909,43 +2911,43 @@
         <v>46</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.019594157599028E+24</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>4.7477623599502562E+25</v>
       </c>
       <c r="K51" s="1">
-        <f t="shared" si="11"/>
-        <v>7.7652241509929693E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.6142240148329752E-2</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" si="12"/>
-        <v>0.92089423903697309</v>
+        <f t="shared" si="6"/>
+        <v>0.93947368421052624</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="13"/>
-        <v>0.92089423903697309</v>
+        <f t="shared" si="6"/>
+        <v>0.93947368421052624</v>
       </c>
       <c r="N51" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q51)</f>
         <v>1</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="15"/>
-        <v>118.59209999999997</v>
+        <f>POWER(H$2,$Q51)</f>
+        <v>35.936999999999998</v>
       </c>
       <c r="P51" s="1">
-        <f t="shared" si="16"/>
-        <v>118.59209999999997</v>
+        <f>POWER(I$2,$Q51)</f>
+        <v>35.936999999999998</v>
       </c>
       <c r="Q51" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R51" s="1">
         <v>46</v>
@@ -2956,43 +2958,43 @@
         <v>47</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>3.3646607200767922E+24</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>1.6004081859843526E+26</v>
       </c>
       <c r="K52" s="1">
-        <f t="shared" si="11"/>
-        <v>2.6175548300574062E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.8122049844537892E-2</v>
       </c>
       <c r="L52" s="1">
-        <f t="shared" si="12"/>
-        <v>0.94067067927773018</v>
+        <f t="shared" si="6"/>
+        <v>0.95964912280701764</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="13"/>
-        <v>0.94067067927773018</v>
+        <f t="shared" si="6"/>
+        <v>0.95964912280701764</v>
       </c>
       <c r="N52" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q52)</f>
         <v>1</v>
       </c>
       <c r="O52" s="1">
-        <f t="shared" si="15"/>
-        <v>35.936999999999998</v>
+        <f>POWER(H$2,$Q52)</f>
+        <v>10.889999999999999</v>
       </c>
       <c r="P52" s="1">
-        <f t="shared" si="16"/>
-        <v>35.936999999999998</v>
+        <f>POWER(I$2,$Q52)</f>
+        <v>10.889999999999999</v>
       </c>
       <c r="Q52" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R52" s="1">
         <v>47</v>
@@ -3003,43 +3005,43 @@
         <v>48</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.1103380376253414E+25</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>5.392380817510898E+26</v>
       </c>
       <c r="K53" s="1">
-        <f t="shared" si="11"/>
-        <v>8.8195327779475377E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.29691653375863908</v>
       </c>
       <c r="L53" s="1">
-        <f t="shared" si="12"/>
-        <v>0.9604471195184866</v>
+        <f t="shared" si="6"/>
+        <v>0.97982456140350882</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" si="13"/>
-        <v>0.9604471195184866</v>
+        <f t="shared" si="6"/>
+        <v>0.97982456140350882</v>
       </c>
       <c r="N53" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q53)</f>
         <v>1</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" si="15"/>
-        <v>10.889999999999999</v>
+        <f>POWER(H$2,$Q53)</f>
+        <v>3.3</v>
       </c>
       <c r="P53" s="1">
-        <f t="shared" si="16"/>
-        <v>10.889999999999999</v>
+        <f>POWER(I$2,$Q53)</f>
+        <v>3.3</v>
       </c>
       <c r="Q53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R53" s="1">
         <v>48</v>
@@ -3050,96 +3052,66 @@
         <v>49</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>3.6641155241636263E+25</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>1.8161268250202324E+27</v>
       </c>
       <c r="K54" s="1">
-        <f t="shared" si="11"/>
-        <v>0.29703744235128587</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="L54" s="1">
-        <f t="shared" si="12"/>
-        <v>0.98022355975924336</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="M54" s="1">
-        <f t="shared" si="13"/>
-        <v>0.98022355975924336</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="N54" s="1">
-        <f t="shared" si="14"/>
+        <f>POWER(G$2,$Q54)</f>
         <v>1</v>
       </c>
       <c r="O54" s="1">
-        <f t="shared" si="15"/>
-        <v>3.3</v>
+        <f>POWER(H$2,$Q54)</f>
+        <v>1</v>
       </c>
       <c r="P54" s="1">
-        <f t="shared" si="16"/>
-        <v>3.3</v>
+        <f>POWER(I$2,$Q54)</f>
+        <v>1</v>
       </c>
       <c r="Q54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R54" s="1">
         <v>49</v>
       </c>
     </row>
     <row r="55" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="F55" s="1">
-        <v>50</v>
-      </c>
-      <c r="G55" s="1">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="H55" s="1">
-        <f t="shared" si="17"/>
-        <v>1.2091581229739966E+26</v>
-      </c>
-      <c r="I55" s="1">
-        <f t="shared" si="18"/>
-        <v>6.1141343348641664E+27</v>
-      </c>
-      <c r="K55" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="L55" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="M55" s="1">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="N55" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="O55" s="1">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="P55" s="1">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="Q55" s="1">
-        <v>0</v>
-      </c>
-      <c r="R55" s="1">
-        <v>50</v>
-      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q5:Q54">
+    <sortCondition descending="1" ref="Q5"/>
+  </sortState>
   <dataValidations count="4">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C13 C3:D3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0.33,0.60,0.15,0.25"</formula1>

</xml_diff>